<commit_message>
added a way to display study sets
</commit_message>
<xml_diff>
--- a/WebApplikacija/WebApplikacija/Data/data.xlsx
+++ b/WebApplikacija/WebApplikacija/Data/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -65,13 +65,23 @@
   </si>
   <si>
     <t>yhh</t>
+  </si>
+  <si>
+    <t>2023-09-28 21:41:51 7_5_8829598</t>
+  </si>
+  <si>
+    <t>dddfdss</t>
+  </si>
+  <si>
+    <t>sdfsd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
@@ -138,7 +148,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -199,6 +209,17 @@
       </c>
       <c r="C5" s="0" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="1048569" ht="12.8"/>

</xml_diff>